<commit_message>
TOR-012 Update data sheets
</commit_message>
<xml_diff>
--- a/data/MissionRosters.xlsx
+++ b/data/MissionRosters.xlsx
@@ -119,13 +119,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -145,10 +149,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -207,19 +211,65 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>